<commit_message>
Recap souris + bib
</commit_message>
<xml_diff>
--- a/Recap Souris.xlsx
+++ b/Recap Souris.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Cours\M2\Stage M2\Rapport\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="0" windowWidth="30855" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="56">
   <si>
     <t>F</t>
   </si>
@@ -53,9 +48,6 @@
     <t>Reçu le</t>
   </si>
   <si>
-    <t>NeuN</t>
-  </si>
-  <si>
     <t>qPCR</t>
   </si>
   <si>
@@ -86,9 +78,6 @@
     <t>Age (jours)</t>
   </si>
   <si>
-    <t>Moyenne Age sacrifice</t>
-  </si>
-  <si>
     <t>Origine</t>
   </si>
   <si>
@@ -162,13 +151,49 @@
   </si>
   <si>
     <t>Prévue</t>
+  </si>
+  <si>
+    <t>Moy Age sacrifice (jour)</t>
+  </si>
+  <si>
+    <t>Mâle</t>
+  </si>
+  <si>
+    <t>Femelle</t>
+  </si>
+  <si>
+    <t>NeuN/MuSK</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>Prévu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,8 +297,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,12 +327,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,7 +387,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,8 +417,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,19 +494,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -482,7 +512,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -511,13 +541,13 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -530,8 +560,31 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -546,6 +599,8 @@
     <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -560,36 +615,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -938,261 +968,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="7" max="8" width="10.875" style="16"/>
-    <col min="10" max="10" width="20.625" customWidth="1"/>
-    <col min="13" max="13" width="44.875" style="13" customWidth="1"/>
-    <col min="14" max="14" width="13.375" customWidth="1"/>
-    <col min="15" max="15" width="21.125" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="16"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="44.83203125" style="13" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:22" s="58" customFormat="1" ht="18">
+      <c r="A1" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="9" t="s">
+      <c r="N1" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="59"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="39">
+        <v>415</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="40">
+        <v>42907</v>
+      </c>
+      <c r="E2" s="40">
+        <v>43123</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41">
+        <f t="shared" ref="G2:G27" ca="1" si="0">IF(F2, F2-D2, TODAY()-D2)</f>
+        <v>264</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="26"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
-        <v>415</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="42">
-        <v>42907</v>
-      </c>
-      <c r="E2" s="42">
-        <v>43123</v>
-      </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43">
-        <f t="shared" ref="G2:G24" ca="1" si="0">IF(F2, F2-D2, TODAY()-D2)</f>
-        <v>261</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="3">
-        <f>COUNTIFS(B:B, "F",C:C, P1)</f>
-        <v>4</v>
-      </c>
-      <c r="Q2" s="3">
-        <f>COUNTIFS(B:B, "F",C:C,Q1)</f>
-        <v>5</v>
-      </c>
-      <c r="R2" s="5">
-        <f>SUM(P2:Q2)</f>
-        <v>9</v>
-      </c>
-      <c r="S2" s="26"/>
+      <c r="S2" s="25" t="s">
+        <v>12</v>
+      </c>
       <c r="T2" s="26"/>
       <c r="U2" s="26"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+      <c r="V2" s="26"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="43">
         <v>417</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="42">
+      <c r="C3" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="40">
         <v>42962</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="40">
         <v>43123</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43">
-        <f t="shared" ca="1" si="0"/>
-        <v>206</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="3">
-        <f>COUNTIFS(B:B, "M",C:C, P1)</f>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>209</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q2)</f>
         <v>4</v>
       </c>
-      <c r="Q3" s="3">
-        <f>COUNTIFS(B:B, "M",C:C,Q1)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <f>SUM(P3:Q3)</f>
-        <v>4</v>
-      </c>
-      <c r="S3" s="26"/>
+      <c r="R3" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R2)</f>
+        <v>5</v>
+      </c>
+      <c r="S3" s="5">
+        <f>SUM(Q3:R3)</f>
+        <v>9</v>
+      </c>
       <c r="T3" s="26"/>
       <c r="U3" s="26"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="41">
+      <c r="V3" s="26"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="39">
         <v>422</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="42">
+      <c r="C4" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="40">
         <v>42962</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="40">
         <v>43123</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="43">
-        <f t="shared" ca="1" si="0"/>
-        <v>206</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="5">
-        <f>SUM(P2:P3)</f>
-        <v>8</v>
-      </c>
-      <c r="Q4" s="5">
-        <f>SUM(Q2:Q3)</f>
-        <v>5</v>
-      </c>
-      <c r="R4" s="5">
-        <f>SUM(R2:R3)</f>
-        <v>13</v>
-      </c>
-      <c r="S4" s="26"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>209</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q2)</f>
+        <v>4</v>
+      </c>
+      <c r="R4" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R2)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <f>SUM(Q4:R4)</f>
+        <v>4</v>
+      </c>
       <c r="T4" s="26"/>
       <c r="U4" s="26"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
+      <c r="V4" s="26"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="43">
         <v>425</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="42">
+      <c r="C5" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="40">
         <v>42964</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="40">
         <v>43123</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43">
-        <f t="shared" ca="1" si="0"/>
-        <v>204</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="26"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>207</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>SUM(Q3:Q4)</f>
+        <v>8</v>
+      </c>
+      <c r="R5" s="5">
+        <f>SUM(R3:R4)</f>
+        <v>5</v>
+      </c>
+      <c r="S5" s="5">
+        <f>SUM(S3:S4)</f>
+        <v>13</v>
+      </c>
       <c r="T5" s="26"/>
       <c r="U5" s="26"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" s="26"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="4">
         <v>435</v>
       </c>
@@ -1200,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f>$P$1</f>
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D6" s="8">
@@ -1212,35 +1251,25 @@
       <c r="F6" s="8">
         <v>43124</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="30">
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>22</v>
+      <c r="H6" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="O6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" s="3">
-        <f>COUNTIFS(C:C, P1,M:M, O6)</f>
-        <v>2</v>
-      </c>
-      <c r="Q6" s="3">
-        <f>COUNTIFS(C:C, Q1,M:M, O6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="10">
         <v>437</v>
       </c>
@@ -1248,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="10" t="str">
-        <f>$Q$1</f>
+        <f>$R$2</f>
         <v>WT</v>
       </c>
       <c r="D7" s="11">
@@ -1265,19 +1294,31 @@
         <v>27</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M7" s="12"/>
+      <c r="N7" s="6"/>
+      <c r="P7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>COUNTIFS(N:N, P7,C:C, Q2,N:N, P7)</f>
+        <v>2</v>
+      </c>
+      <c r="R7" s="3">
+        <f>COUNTIFS(N:N, P7,C:C, R2,N:N, P7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="10">
         <v>440</v>
       </c>
@@ -1285,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="10" t="str">
-        <f t="shared" ref="C8:C9" si="1">$Q$1</f>
+        <f>$R$2</f>
         <v>WT</v>
       </c>
       <c r="D8" s="11">
@@ -1302,7 +1343,7 @@
         <v>36</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -1310,16 +1351,10 @@
         <v>7</v>
       </c>
       <c r="L8" s="12"/>
-      <c r="M8" s="6"/>
-      <c r="O8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="18">
-        <f ca="1">IF(G:G="E", "", AVERAGEIF(F:F, "&lt;&gt;",G:G))</f>
-        <v>32.363636363636367</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M8" s="12"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="10">
         <v>441</v>
       </c>
@@ -1327,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f>$R$2</f>
         <v>WT</v>
       </c>
       <c r="D9" s="11">
@@ -1344,25 +1379,33 @@
         <v>35</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="18">
+        <f ca="1">IF(G:G="E", "", AVERAGEIF(F:F, "&lt;&gt;",G:G))</f>
+        <v>32.363636363636367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="2">
         <v>439</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="28" t="str">
-        <f>$P$1</f>
+      <c r="C10" s="7" t="str">
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D10" s="14">
@@ -1374,26 +1417,27 @@
       <c r="F10" s="14">
         <v>43146</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>22</v>
+      <c r="H10" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+      <c r="N10" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="19">
         <v>443</v>
       </c>
@@ -1401,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f t="shared" ref="C11:C12" si="2">$P$1</f>
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D11" s="14">
@@ -1413,32 +1457,33 @@
       <c r="F11" s="14">
         <v>43146</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
-      <c r="H11" s="33" t="s">
-        <v>22</v>
+      <c r="H11" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="7">
         <v>442</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="28" t="str">
-        <f t="shared" si="2"/>
+      <c r="C12" s="7" t="str">
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D12" s="8">
@@ -1450,12 +1495,12 @@
       <c r="F12" s="8">
         <v>43146</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="30">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
-      <c r="H12" s="32" t="s">
-        <v>22</v>
+      <c r="H12" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>7</v>
@@ -1464,8 +1509,12 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N12" s="5"/>
+      <c r="P12" s="51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="10">
         <v>1</v>
       </c>
@@ -1473,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="20">
         <v>43130</v>
@@ -1489,19 +1538,23 @@
         <v>35</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="10">
         <v>2</v>
       </c>
@@ -1509,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="20">
         <v>43130</v>
@@ -1525,19 +1578,23 @@
         <v>35</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="10">
         <v>3</v>
       </c>
@@ -1545,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="20">
         <v>43130</v>
@@ -1561,19 +1618,20 @@
         <v>35</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="10">
         <v>4</v>
       </c>
@@ -1581,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="20">
         <v>43130</v>
@@ -1597,27 +1655,28 @@
         <v>35</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="7">
         <v>444</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="28" t="str">
-        <f>$P$1</f>
+      <c r="C17" s="7" t="str">
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D17" s="8">
@@ -1627,30 +1686,33 @@
         <v>43166</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="32">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>22</v>
+      <c r="G17" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="7">
         <v>445</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="28" t="str">
-        <f t="shared" ref="C18:C19" si="3">$P$1</f>
+      <c r="C18" s="7" t="str">
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D18" s="8">
@@ -1660,22 +1722,25 @@
         <v>43166</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="32">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>22</v>
+      <c r="G18" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="4">
         <v>448</v>
       </c>
@@ -1683,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D19" s="8">
@@ -1693,54 +1758,58 @@
         <v>43166</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="32">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>22</v>
+      <c r="G19" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="41">
+        <v>55</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="39">
         <v>449</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="42">
+      <c r="C20" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="40">
         <v>43132</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="40">
         <v>43166</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="43">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="H20" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="40"/>
+      <c r="G20" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="10">
         <v>450</v>
       </c>
@@ -1748,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="10" t="str">
-        <f>$Q$1</f>
+        <f>$R$2</f>
         <v>WT</v>
       </c>
       <c r="D21" s="11">
@@ -1760,52 +1829,56 @@
       <c r="F21" s="11"/>
       <c r="G21" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="41">
+        <v>55</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="39">
         <v>451</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="42">
+      <c r="C22" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="40">
         <v>43132</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="40">
         <v>43166</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="H22" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="40"/>
+      <c r="G22" s="41">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="10">
         <v>455</v>
       </c>
@@ -1813,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="10" t="str">
-        <f>$Q$1</f>
+        <f>$R$2</f>
         <v>WT</v>
       </c>
       <c r="D23" s="11">
@@ -1825,20 +1898,23 @@
       <c r="F23" s="11"/>
       <c r="G23" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="4">
         <v>457</v>
       </c>
@@ -1846,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="4" t="str">
-        <f>$P$1</f>
+        <f>$Q$2</f>
         <v>Mut</v>
       </c>
       <c r="D24" s="8">
@@ -1856,236 +1932,398 @@
         <v>43166</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="32">
-        <f t="shared" ca="1" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>22</v>
+      <c r="G24" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="54">
+        <v>43147</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="54">
+        <v>43150</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="54">
+        <v>43150</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="30">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="35">
+        <v>43166</v>
+      </c>
+      <c r="E28" s="35">
+        <v>43166</v>
+      </c>
+      <c r="F28" s="38"/>
+      <c r="G28" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="48">
+        <v>43166</v>
+      </c>
+      <c r="E29" s="48">
+        <v>43166</v>
+      </c>
+      <c r="F29" s="47"/>
+      <c r="G29" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="B30" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="48">
+        <v>43166</v>
+      </c>
+      <c r="E30" s="48">
+        <v>43166</v>
+      </c>
+      <c r="F30" s="47"/>
+      <c r="G30" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="48">
+        <v>43166</v>
+      </c>
+      <c r="E31" s="48">
+        <v>43166</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="23">
+        <v>43166</v>
+      </c>
+      <c r="E32" s="23">
+        <v>43166</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="48">
+        <v>43166</v>
+      </c>
+      <c r="E33" s="48">
+        <v>43166</v>
+      </c>
+      <c r="F33" s="47"/>
+      <c r="G33" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="37">
+      <c r="D34" s="35">
         <v>43166</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50">
+      <c r="E34" s="35">
         <v>43166</v>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50">
-        <v>43166</v>
-      </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50">
-        <v>43166</v>
-      </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="30" t="s">
+      <c r="F34" s="34"/>
+      <c r="G34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="54">
+        <v>43168</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="30">
+        <f ca="1">IF(F35, F35-D35, TODAY()-D35)</f>
         <v>3</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23">
-        <v>43166</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50">
-        <v>43166</v>
-      </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37">
-        <v>43166</v>
-      </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="H35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="54">
+        <v>43168</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="30">
+        <f ca="1">IF(F36, F36-D36, TODAY()-D36)</f>
+        <v>3</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="54">
+        <v>43168</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="30">
+        <f ca="1">IF(F37, F37-D37, TODAY()-D37)</f>
+        <v>3</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="12"/>
     </row>
   </sheetData>
-  <sortState ref="A2:M24">
-    <sortCondition ref="D2:D24"/>
+  <sortState ref="A2:M37">
+    <sortCondition ref="D2:D37"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="A1:M1048576">
+  <conditionalFormatting sqref="A1:N1048576">
     <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>$C$2="Mut"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Reprise intro, modif souris
</commit_message>
<xml_diff>
--- a/Recap Souris.xlsx
+++ b/Recap Souris.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="52">
   <si>
     <t>F</t>
   </si>
@@ -159,12 +159,6 @@
     <t>1+ : Origine P5</t>
   </si>
   <si>
-    <t>100+ : Origine Pascale</t>
-  </si>
-  <si>
-    <t>400+ : Origine ICM</t>
-  </si>
-  <si>
     <t>200+ : Embryon</t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>Coupés cryostats 20µ, peu concluant. -20°C</t>
+  </si>
+  <si>
+    <t>100+ : Pascale</t>
+  </si>
+  <si>
+    <t>400+ : ICM</t>
   </si>
 </sst>
 </file>
@@ -387,8 +387,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -675,7 +685,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="87">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -714,6 +724,11 @@
     <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -752,139 +767,14 @@
     <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -1233,11 +1123,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1246,7 +1136,7 @@
     <col min="10" max="10" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" customWidth="1"/>
     <col min="14" max="14" width="36.5" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
     <col min="16" max="16" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1316,8 +1206,8 @@
       </c>
       <c r="F2" s="50"/>
       <c r="G2" s="51">
-        <f ca="1">IF(F2, F2-D2, TODAY()-D2)</f>
-        <v>274</v>
+        <f t="shared" ref="G2:G30" ca="1" si="0">IF(F2, F2-D2, TODAY()-D2)</f>
+        <v>275</v>
       </c>
       <c r="H2" s="51" t="s">
         <v>19</v>
@@ -1330,7 +1220,12 @@
       <c r="N2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="Q2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="26" t="str">
-        <f t="shared" ref="C3:C5" si="0">$T$2</f>
+        <f t="shared" ref="C3:C5" si="1">$T$2</f>
         <v>Het</v>
       </c>
       <c r="D3" s="62">
@@ -1365,8 +1260,8 @@
       </c>
       <c r="F3" s="62"/>
       <c r="G3" s="63">
-        <f ca="1">IF(F3, F3-D3, TODAY()-D3)</f>
-        <v>219</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>220</v>
       </c>
       <c r="H3" s="63" t="s">
         <v>19</v>
@@ -1379,6 +1274,9 @@
       <c r="N3" s="27" t="s">
         <v>28</v>
       </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
       <c r="P3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1409,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Het</v>
       </c>
       <c r="D4" s="50">
@@ -1420,8 +1318,8 @@
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="51">
-        <f ca="1">IF(F4, F4-D4, TODAY()-D4)</f>
-        <v>219</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>220</v>
       </c>
       <c r="H4" s="51" t="s">
         <v>19</v>
@@ -1434,6 +1332,9 @@
       <c r="N4" s="27" t="s">
         <v>28</v>
       </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
       <c r="P4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1464,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Het</v>
       </c>
       <c r="D5" s="62">
@@ -1475,8 +1376,8 @@
       </c>
       <c r="F5" s="62"/>
       <c r="G5" s="63">
-        <f ca="1">IF(F5, F5-D5, TODAY()-D5)</f>
-        <v>217</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>218</v>
       </c>
       <c r="H5" s="63" t="s">
         <v>19</v>
@@ -1489,6 +1390,9 @@
       <c r="N5" s="27" t="s">
         <v>28</v>
       </c>
+      <c r="O5" t="s">
+        <v>46</v>
+      </c>
       <c r="P5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1532,7 +1436,7 @@
         <v>43124</v>
       </c>
       <c r="G6" s="53">
-        <f ca="1">IF(F6, F6-D6, TODAY()-D6)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
       <c r="H6" s="53" t="s">
@@ -1548,6 +1452,9 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
+      <c r="O6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="9">
@@ -1570,7 +1477,7 @@
         <v>43124</v>
       </c>
       <c r="G7" s="55">
-        <f ca="1">IF(F7, F7-D7, TODAY()-D7)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
       <c r="H7" s="55" t="s">
@@ -1586,16 +1493,17 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="6"/>
-      <c r="P7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="3">
-        <f>COUNTIFS(N:N, P7,C:C, Q2,N:N, P7)</f>
+      <c r="P7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="R7" s="3">
-        <f>COUNTIFS(N:N, P7,C:C, R2,N:N, P7)</f>
-        <v>1</v>
+      <c r="R7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" s="17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1619,7 +1527,7 @@
         <v>43146</v>
       </c>
       <c r="G8" s="67">
-        <f ca="1">IF(F8, F8-D8, TODAY()-D8)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H8" s="67" t="s">
@@ -1637,6 +1545,21 @@
       <c r="N8" s="22" t="s">
         <v>15</v>
       </c>
+      <c r="P8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q7,I:I, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="R8" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R7,I:I, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="S8" s="5">
+        <f>SUM(Q8:R8)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="9">
@@ -1659,7 +1582,7 @@
         <v>43147</v>
       </c>
       <c r="G9" s="55">
-        <f ca="1">IF(F9, F9-D9, TODAY()-D9)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>36</v>
       </c>
       <c r="H9" s="55" t="s">
@@ -1673,12 +1596,20 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="6"/>
-      <c r="P9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="14">
-        <f ca="1">IF(G:G="E", "", AVERAGEIF(F:F, "&lt;&gt;",G:G))</f>
-        <v>31.857142857142858</v>
+      <c r="P9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q7,I:I, "&lt;&gt;")</f>
+        <v>2</v>
+      </c>
+      <c r="R9" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R7,I:I, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="S9" s="5">
+        <f>SUM(Q9:R9)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1702,7 +1633,7 @@
         <v>43146</v>
       </c>
       <c r="G10" s="73">
-        <f ca="1">IF(F10, F10-D10, TODAY()-D10)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H10" s="73" t="s">
@@ -1714,7 +1645,22 @@
       <c r="L10" s="74"/>
       <c r="M10" s="74"/>
       <c r="N10" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>SUM(Q8:Q9)</f>
+        <v>3</v>
+      </c>
+      <c r="R10" s="5">
+        <f>SUM(R8:R9)</f>
+        <v>2</v>
+      </c>
+      <c r="S10" s="5">
+        <f>SUM(S8:S9)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1738,7 +1684,7 @@
         <v>43146</v>
       </c>
       <c r="G11" s="65">
-        <f ca="1">IF(F11, F11-D11, TODAY()-D11)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
       <c r="H11" s="65" t="s">
@@ -1752,13 +1698,6 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="P11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11" s="10">
-        <f>COUNTIF(A:A, "&lt;&gt;")-1</f>
-        <v>38</v>
-      </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="4">
@@ -1781,7 +1720,7 @@
         <v>43146</v>
       </c>
       <c r="G12" s="53">
-        <f ca="1">IF(F12, F12-D12, TODAY()-D12)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
       <c r="H12" s="53" t="s">
@@ -1797,6 +1736,18 @@
       <c r="N12" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="P12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="46">
@@ -1818,7 +1769,7 @@
         <v>43165</v>
       </c>
       <c r="G13" s="57">
-        <f ca="1">IF(F13, F13-D13, TODAY()-D13)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H13" s="47" t="s">
@@ -1834,8 +1785,20 @@
       <c r="N13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="39" t="s">
-        <v>37</v>
+      <c r="P13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q12)</f>
+        <v>4</v>
+      </c>
+      <c r="R13" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R12)</f>
+        <v>5</v>
+      </c>
+      <c r="S13" s="5">
+        <f>SUM(Q13:R13)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1858,7 +1821,7 @@
         <v>43165</v>
       </c>
       <c r="G14" s="57">
-        <f ca="1">IF(F14, F14-D14, TODAY()-D14)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H14" s="47" t="s">
@@ -1874,8 +1837,20 @@
       <c r="N14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="40" t="s">
-        <v>38</v>
+      <c r="P14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q12)</f>
+        <v>4</v>
+      </c>
+      <c r="R14" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R12)</f>
+        <v>2</v>
+      </c>
+      <c r="S14" s="5">
+        <f>SUM(Q14:R14)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -1898,7 +1873,7 @@
         <v>43165</v>
       </c>
       <c r="G15" s="57">
-        <f ca="1">IF(F15, F15-D15, TODAY()-D15)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H15" s="47" t="s">
@@ -1914,8 +1889,20 @@
       <c r="N15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P15" s="42" t="s">
-        <v>29</v>
+      <c r="P15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>SUM(Q13:Q14)</f>
+        <v>8</v>
+      </c>
+      <c r="R15" s="5">
+        <f>SUM(R13:R14)</f>
+        <v>7</v>
+      </c>
+      <c r="S15" s="5">
+        <f>SUM(S13:S14)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1938,7 +1925,7 @@
         <v>43165</v>
       </c>
       <c r="G16" s="57">
-        <f ca="1">IF(F16, F16-D16, TODAY()-D16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="H16" s="47" t="s">
@@ -1954,11 +1941,8 @@
       <c r="N16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P16" s="46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="7">
         <v>444</v>
       </c>
@@ -1977,8 +1961,8 @@
       </c>
       <c r="F17" s="66"/>
       <c r="G17" s="67">
-        <f ca="1">IF(F17, F17-D17, TODAY()-D17)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H17" s="67" t="s">
         <v>19</v>
@@ -1993,8 +1977,20 @@
       <c r="N17" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="P17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="7">
         <v>445</v>
       </c>
@@ -2013,8 +2009,8 @@
       </c>
       <c r="F18" s="66"/>
       <c r="G18" s="67">
-        <f ca="1">IF(F18, F18-D18, TODAY()-D18)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H18" s="67" t="s">
         <v>19</v>
@@ -2030,10 +2026,22 @@
         <v>23</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q17)</f>
+        <v>4</v>
+      </c>
+      <c r="R18" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R17)</f>
+        <v>5</v>
+      </c>
+      <c r="S18" s="5">
+        <f>SUM(Q18:R18)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="4">
         <v>448</v>
       </c>
@@ -2052,8 +2060,8 @@
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="53">
-        <f ca="1">IF(F19, F19-D19, TODAY()-D19)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H19" s="53" t="s">
         <v>19</v>
@@ -2068,11 +2076,23 @@
       <c r="N19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="P19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q17)</f>
+        <v>4</v>
+      </c>
+      <c r="R19" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R17)</f>
+        <v>2</v>
+      </c>
+      <c r="S19" s="5">
+        <f>SUM(Q19:R19)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="26">
         <v>449</v>
       </c>
@@ -2091,8 +2111,8 @@
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="51">
-        <f ca="1">IF(F20, F20-D20, TODAY()-D20)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H20" s="51" t="s">
         <v>19</v>
@@ -2105,11 +2125,23 @@
       <c r="N20" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P20" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="P20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>SUM(Q18:Q19)</f>
+        <v>8</v>
+      </c>
+      <c r="R20" s="5">
+        <f>SUM(R18:R19)</f>
+        <v>7</v>
+      </c>
+      <c r="S20" s="5">
+        <f>SUM(S18:S19)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="9">
         <v>450</v>
       </c>
@@ -2128,8 +2160,8 @@
       </c>
       <c r="F21" s="54"/>
       <c r="G21" s="55">
-        <f ca="1">IF(F21, F21-D21, TODAY()-D21)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H21" s="55" t="s">
         <v>19</v>
@@ -2145,7 +2177,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:19">
       <c r="A22" s="26">
         <v>451</v>
       </c>
@@ -2164,8 +2196,8 @@
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="51">
-        <f ca="1">IF(F22, F22-D22, TODAY()-D22)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="H22" s="51" t="s">
         <v>19</v>
@@ -2178,9 +2210,20 @@
       <c r="N22" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="Q22" s="45"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="P22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S22" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="9">
         <v>455</v>
       </c>
@@ -2199,8 +2242,8 @@
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="55">
-        <f ca="1">IF(F23, F23-D23, TODAY()-D23)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="H23" s="55" t="s">
         <v>19</v>
@@ -2215,12 +2258,23 @@
       <c r="N23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P23" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="41"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="P23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q22)</f>
+        <v>4</v>
+      </c>
+      <c r="R23" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R22)</f>
+        <v>5</v>
+      </c>
+      <c r="S23" s="5">
+        <f>SUM(Q23:R23)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="4">
         <v>457</v>
       </c>
@@ -2239,8 +2293,8 @@
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="53">
-        <f ca="1">IF(F24, F24-D24, TODAY()-D24)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="H24" s="53" t="s">
         <v>19</v>
@@ -2255,12 +2309,23 @@
       <c r="N24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P24" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q24" s="41"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="P24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q22)</f>
+        <v>4</v>
+      </c>
+      <c r="R24" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R22)</f>
+        <v>2</v>
+      </c>
+      <c r="S24" s="5">
+        <f>SUM(Q24:R24)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="28">
         <v>1</v>
       </c>
@@ -2279,8 +2344,8 @@
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="63">
-        <f ca="1">IF(F25, F25-D25, TODAY()-D25)</f>
-        <v>34</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>40</v>
@@ -2290,13 +2355,26 @@
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="P25" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q25" s="45"/>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="N25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>SUM(Q23:Q24)</f>
+        <v>8</v>
+      </c>
+      <c r="R25" s="5">
+        <f>SUM(R23:R24)</f>
+        <v>7</v>
+      </c>
+      <c r="S25" s="5">
+        <f>SUM(S23:S24)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="39">
         <v>2</v>
       </c>
@@ -2315,8 +2393,8 @@
       </c>
       <c r="F26" s="68"/>
       <c r="G26" s="69">
-        <f ca="1">IF(F26, F26-D26, TODAY()-D26)</f>
-        <v>31</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="H26" s="39" t="s">
         <v>40</v>
@@ -2329,11 +2407,8 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="P26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="26">
         <v>3</v>
       </c>
@@ -2352,8 +2427,8 @@
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="51">
-        <f ca="1">IF(F27, F27-D27, TODAY()-D27)</f>
-        <v>31</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>40</v>
@@ -2363,12 +2438,23 @@
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="P27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="N27" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S27" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="47">
         <v>105</v>
       </c>
@@ -2388,7 +2474,7 @@
         <v>43180</v>
       </c>
       <c r="G28" s="57">
-        <f ca="1">IF(F28, F28-D28, TODAY()-D28)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="H28" s="47" t="s">
@@ -2402,10 +2488,25 @@
       </c>
       <c r="M28" s="12"/>
       <c r="N28" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>48</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="3">
+        <f>COUNTIFS(B:B, "F",C:C, Q27)</f>
+        <v>4</v>
+      </c>
+      <c r="R28" s="3">
+        <f>COUNTIFS(B:B, "F",C:C,R27)</f>
+        <v>5</v>
+      </c>
+      <c r="S28" s="5">
+        <f>SUM(Q28:R28)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="47">
         <v>106</v>
       </c>
@@ -2425,7 +2526,7 @@
         <v>43180</v>
       </c>
       <c r="G29" s="57">
-        <f ca="1">IF(F29, F29-D29, TODAY()-D29)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="H29" s="47" t="s">
@@ -2439,10 +2540,25 @@
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>48</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q29" s="3">
+        <f>COUNTIFS(B:B, "M",C:C, Q27)</f>
+        <v>4</v>
+      </c>
+      <c r="R29" s="3">
+        <f>COUNTIFS(B:B, "M",C:C,R27)</f>
+        <v>2</v>
+      </c>
+      <c r="S29" s="5">
+        <f>SUM(Q29:R29)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="47">
         <v>107</v>
       </c>
@@ -2462,7 +2578,7 @@
         <v>43180</v>
       </c>
       <c r="G30" s="57">
-        <f ca="1">IF(F30, F30-D30, TODAY()-D30)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="H30" s="47" t="s">
@@ -2476,10 +2592,25 @@
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>48</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q30" s="5">
+        <f>SUM(Q28:Q29)</f>
+        <v>8</v>
+      </c>
+      <c r="R30" s="5">
+        <f>SUM(R28:R29)</f>
+        <v>7</v>
+      </c>
+      <c r="S30" s="5">
+        <f>SUM(S28:S29)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="23">
         <v>201</v>
       </c>
@@ -2514,7 +2645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:19">
       <c r="A32" s="34">
         <v>202</v>
       </c>
@@ -2548,8 +2679,19 @@
       <c r="N32" s="38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q32" s="3">
+        <f>COUNTIFS(N:N, P32,C:C, Q2,N:N, P32)</f>
+        <v>2</v>
+      </c>
+      <c r="R32" s="3">
+        <f>COUNTIFS(N:N, P32,C:C, R2,N:N, P32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="34">
         <v>203</v>
       </c>
@@ -2557,7 +2699,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="36" t="str">
-        <f t="shared" ref="C33:C34" si="1">$T$2</f>
+        <f t="shared" ref="C33:C34" si="2">$T$2</f>
         <v>Het</v>
       </c>
       <c r="D33" s="60">
@@ -2584,7 +2726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:17">
       <c r="A34" s="34">
         <v>204</v>
       </c>
@@ -2592,7 +2734,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Het</v>
       </c>
       <c r="D34" s="60">
@@ -2618,8 +2760,15 @@
       <c r="N34" s="38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="P34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q34" s="14">
+        <f ca="1">IF(G:G="E", "", AVERAGEIF(F:F, "&lt;&gt;",G:G))</f>
+        <v>31.857142857142858</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="19">
         <v>205</v>
       </c>
@@ -2654,7 +2803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:17">
       <c r="A36" s="34">
         <v>206</v>
       </c>
@@ -2688,8 +2837,15 @@
       <c r="N36" s="38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="P36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q36" s="10">
+        <f>COUNTIF(A:A, "&lt;&gt;")-1</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="23">
         <v>207</v>
       </c>
@@ -2724,7 +2880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:17">
       <c r="A38" s="39">
         <v>4</v>
       </c>
@@ -2744,7 +2900,7 @@
       <c r="F38" s="39"/>
       <c r="G38" s="67">
         <f ca="1">IF(F38, F38-D38, TODAY()-D38)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H38" s="39" t="s">
         <v>40</v>
@@ -2755,8 +2911,11 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="P38" s="39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="28">
         <v>5</v>
       </c>
@@ -2776,7 +2935,7 @@
       <c r="F39" s="28"/>
       <c r="G39" s="70">
         <f ca="1">IF(F39, F39-D39, TODAY()-D39)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H39" s="28" t="s">
         <v>40</v>
@@ -2786,7 +2945,49 @@
       <c r="K39" s="27"/>
       <c r="L39" s="27"/>
       <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
+      <c r="N39" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P39" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="P40" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="P41" s="46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="P43" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="P44" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="P45" s="44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="Q47" s="45"/>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="Q48" s="41"/>
+    </row>
+    <row r="49" spans="17:17">
+      <c r="Q49" s="41"/>
+    </row>
+    <row r="50" spans="17:17">
+      <c r="Q50" s="45"/>
     </row>
   </sheetData>
   <sortState ref="A2:N39">
@@ -2794,8 +2995,8 @@
     <sortCondition ref="A2:A39"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="P19:P20 Q23:Q24 G28:N30 A28:D30 A1:N27 A31:N1048576">
-    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="P44:P45 Q48:Q49 G28:N30 A28:D30 A1:N27 A31:N1048576">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>$C$2="Mut"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>